<commit_message>
remove contained subject from FolderComprehensive 9ddb33633488278171c77be70e62953ea9eb758b
</commit_message>
<xml_diff>
--- a/ig/nr-change-contained/StructureDefinition-pdsm-folder-comprehensive.xlsx
+++ b/ig/nr-change-contained/StructureDefinition-pdsm-folder-comprehensive.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-12T08:15:17+00:00</t>
+    <t>2023-07-12T08:17:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -721,7 +721,7 @@
     <t>List.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://interopsante.org/fhir/StructureDefinition/FrPatient) &lt;&lt;contained&gt;&gt;
+    <t xml:space="preserve">Reference(http://interopsante.org/fhir/StructureDefinition/FrPatient)
 </t>
   </si>
   <si>

</xml_diff>